<commit_message>
updates coverage in project metadata excel
</commit_message>
<xml_diff>
--- a/data-raw/metadata/KDL_project_metadata.xlsx
+++ b/data-raw/metadata/KDL_project_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F77418-37E6-9F42-AC70-2BF01B9E87ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5756F6-3618-4F4F-BD59-57C1426C8E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33580" yWindow="2120" windowWidth="30240" windowHeight="17200" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="71">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -274,14 +274,17 @@
   <si>
     <t>Knights Landing Rotary Screw Trap</t>
   </si>
+  <si>
+    <t>2006-10-02</t>
+  </si>
+  <si>
+    <t>2022-10-22</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -363,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -386,13 +389,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -51046,7 +51046,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -51083,7 +51083,7 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B2">
@@ -51098,11 +51098,11 @@
       <c r="E2">
         <v>38.802278000000001</v>
       </c>
-      <c r="F2" s="12">
-        <v>38992</v>
+      <c r="F2" s="13" t="s">
+        <v>69</v>
       </c>
-      <c r="G2" s="13">
-        <v>44699</v>
+      <c r="G2" s="13" t="s">
+        <v>70</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -52136,8 +52136,8 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G2:G8" xr:uid="{00000000-0002-0000-0800-000000000000}">
-      <formula1>F2</formula1>
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showErrorMessage="1" sqref="G3:G8" xr:uid="{00000000-0002-0000-0800-000000000000}">
+      <formula1>F3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
updates license for project metadata to CCBY
</commit_message>
<xml_diff>
--- a/data-raw/metadata/KDL_project_metadata.xlsx
+++ b/data-raw/metadata/KDL_project_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F5756F6-3618-4F4F-BD59-57C1426C8E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424CD2C0-4FF2-9D40-8D6F-9DD17D8D0434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -158,9 +158,6 @@
     <t>intellectual_rights_description</t>
   </si>
   <si>
-    <t>CCO</t>
-  </si>
-  <si>
     <t>organization</t>
   </si>
   <si>
@@ -280,6 +277,9 @@
   <si>
     <t>2022-10-22</t>
   </si>
+  <si>
+    <t>CCBY</t>
+  </si>
 </sst>
 </file>
 
@@ -392,7 +392,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -636,7 +636,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -4670,34 +4670,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -16739,37 +16739,37 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C2" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="C3" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4"/>
     </row>
@@ -20801,10 +20801,10 @@
     </row>
     <row r="2" spans="1:2" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -24866,7 +24866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -24897,7 +24899,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -31929,7 +31931,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>9</v>
@@ -39957,22 +39959,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -47017,18 +47019,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -51045,7 +51047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -51061,30 +51063,30 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2">
         <v>-121.698781</v>
@@ -51099,10 +51101,10 @@
         <v>38.802278000000001</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>

</xml_diff>

<commit_message>
moves project coordinates one mile upstream
</commit_message>
<xml_diff>
--- a/data-raw/metadata/KDL_project_metadata.xlsx
+++ b/data-raw/metadata/KDL_project_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424CD2C0-4FF2-9D40-8D6F-9DD17D8D0434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8EEDBF-1D9F-4443-BF87-16305BD46885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -24866,7 +24866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -51047,8 +51047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -51089,16 +51089,16 @@
         <v>67</v>
       </c>
       <c r="B2">
-        <v>-121.698781</v>
+        <v>-121.692078</v>
       </c>
       <c r="C2">
-        <v>-121.698781</v>
+        <v>-121.692078</v>
       </c>
       <c r="D2">
-        <v>38.802278000000001</v>
+        <v>38.791077000000001</v>
       </c>
       <c r="E2">
-        <v>38.802278000000001</v>
+        <v>38.791077000000001</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
updates coordiantes to bounding box and updates xml
</commit_message>
<xml_diff>
--- a/data-raw/metadata/KDL_project_metadata.xlsx
+++ b/data-raw/metadata/KDL_project_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8EEDBF-1D9F-4443-BF87-16305BD46885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF4AA39-C683-7F47-A8C8-DFC6BFAC442A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -393,6 +393,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -51048,7 +51049,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -51088,17 +51089,17 @@
       <c r="A2" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B2">
-        <v>-121.692078</v>
+      <c r="B2" s="14">
+        <v>-121.712036</v>
       </c>
-      <c r="C2">
-        <v>-121.692078</v>
+      <c r="C2" s="14">
+        <v>-121.680193</v>
       </c>
-      <c r="D2">
-        <v>38.791077000000001</v>
+      <c r="D2" s="14">
+        <v>38.806539999999998</v>
       </c>
-      <c r="E2">
-        <v>38.791077000000001</v>
+      <c r="E2" s="14">
+        <v>38.768673</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
standardizes naming of clean data
</commit_message>
<xml_diff>
--- a/data-raw/metadata/KDL_project_metadata.xlsx
+++ b/data-raw/metadata/KDL_project_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12649E3-0357-AC48-AD3E-2A48A0B7F9FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD01A16-8404-F74A-904D-18FD1B53C862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>Interagency Ecological Program currently funded through California Department of Water Resources and the U.S. Bureau of Reclamation; Past Funding: Interagency Ecological Program funded through California Department of Water Resources</t>
+  </si>
+  <si>
+    <t>SRJPE</t>
+  </si>
+  <si>
+    <t>Chinook salmon</t>
   </si>
 </sst>
 </file>
@@ -21819,7 +21825,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21891,9 +21899,15 @@
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -39948,7 +39962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates information on project metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/KDL_project_metadata.xlsx
+++ b/data-raw/metadata/KDL_project_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B4850E3-E323-4C41-8217-D983450802F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692B657C-3CDE-4DD3-8FCB-7D4998431A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="1360" windowWidth="15000" windowHeight="12550" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="1710" windowWidth="21600" windowHeight="11180" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>orcid</t>
-  </si>
-  <si>
-    <t>principal investigator</t>
   </si>
   <si>
     <t>creator</t>
@@ -242,19 +239,10 @@
     <t>California Department of Fish and Wildlife</t>
   </si>
   <si>
-    <t>Jeanine</t>
-  </si>
-  <si>
-    <t>Phillips</t>
-  </si>
-  <si>
     <t>Nick</t>
   </si>
   <si>
     <t>Bauer</t>
-  </si>
-  <si>
-    <t>jeanine.phillips@wildlife.ca.gov</t>
   </si>
   <si>
     <t xml:space="preserve">nick.bauer@wildlife.ca.gov </t>
@@ -288,6 +276,9 @@
   </si>
   <si>
     <t>Chinook salmon</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -646,7 +637,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -4680,34 +4671,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16714,7 +16705,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -16749,38 +16740,28 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -20778,8 +20759,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{0A3182CE-55B0-8D4E-B1F7-1E69A85A837C}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{9B4CD9CE-9AE5-7249-A818-70FED6214921}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9B4CD9CE-9AE5-7249-A818-70FED6214921}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -20803,18 +20783,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:2" ht="114.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -21838,75 +21818,75 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -24900,24 +24880,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -31925,7 +31905,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -31949,18 +31931,28 @@
         <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -39949,10 +39941,13 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D1" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D1:D2" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"creator,field technician,program founder,other,associate,reviewer,researcher,principal investigator,lab technician"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{1B5DC908-488C-442B-A5DA-DEE73874664E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -39962,7 +39957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -39977,19 +39972,19 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -40014,14 +40009,14 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="B2" s="8">
-        <v>0</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" s="8"/>
     </row>
@@ -46041,18 +46036,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -50085,30 +50080,30 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2" s="14">
         <v>-121.712036</v>
@@ -50123,10 +50118,10 @@
         <v>38.768673</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>

</xml_diff>

<commit_message>
updates date range of project petadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/KDL_project_metadata.xlsx
+++ b/data-raw/metadata/KDL_project_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692B657C-3CDE-4DD3-8FCB-7D4998431A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0B7431-A0CC-4A29-9AE0-0B4AE84E9676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1710" windowWidth="21600" windowHeight="11180" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2000" yWindow="2170" windowWidth="19170" windowHeight="11310" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -260,9 +260,6 @@
     <t>2006-10-02</t>
   </si>
   <si>
-    <t>2022-10-22</t>
-  </si>
-  <si>
     <t>CCBY</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>2024-06-04</t>
   </si>
 </sst>
 </file>
@@ -16705,7 +16705,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -21880,13 +21880,13 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -24897,7 +24897,7 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -31905,7 +31905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -40009,14 +40009,14 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E2" s="8"/>
     </row>
@@ -50064,8 +50064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -50121,7 +50121,7 @@
         <v>63</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>

</xml_diff>

<commit_message>
adds language to metadata, corrects personnel listed
</commit_message>
<xml_diff>
--- a/data-raw/metadata/KDL_project_metadata.xlsx
+++ b/data-raw/metadata/KDL_project_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-knights-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420FBE7C-0566-47A6-85AB-81BE0B2B914D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38846D02-921D-4660-9FEF-48A85C1866CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="1740" windowWidth="19200" windowHeight="11170" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="70">
   <si>
     <t xml:space="preserve">name </t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>orcid</t>
-  </si>
-  <si>
-    <t>principal investigator</t>
   </si>
   <si>
     <t>creator</t>
@@ -242,19 +239,10 @@
     <t>California Department of Fish and Wildlife</t>
   </si>
   <si>
-    <t>Jeanine</t>
-  </si>
-  <si>
-    <t>Phillips</t>
-  </si>
-  <si>
     <t>Nick</t>
   </si>
   <si>
     <t>Bauer</t>
-  </si>
-  <si>
-    <t>jeanine.phillips@wildlife.ca.gov</t>
   </si>
   <si>
     <t xml:space="preserve">nick.bauer@wildlife.ca.gov </t>
@@ -622,7 +610,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -646,7 +634,7 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -4663,8 +4651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4680,34 +4668,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -16713,8 +16701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -16749,38 +16737,28 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>57</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -20778,8 +20756,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{0A3182CE-55B0-8D4E-B1F7-1E69A85A837C}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{9B4CD9CE-9AE5-7249-A818-70FED6214921}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9B4CD9CE-9AE5-7249-A818-70FED6214921}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -20803,18 +20780,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" spans="1:2" ht="114.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -21838,75 +21815,75 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B12" s="2"/>
     </row>
@@ -24900,24 +24877,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -31949,7 +31926,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>9</v>
@@ -39977,19 +39954,19 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -40014,12 +39991,12 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
       <c r="D2" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E2" s="8"/>
     </row>
@@ -46039,18 +46016,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -50068,7 +50045,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -50083,30 +50060,30 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2" s="14">
         <v>-121.712036</v>
@@ -50121,10 +50098,10 @@
         <v>38.768673</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>

</xml_diff>